<commit_message>
Added details for "Splunk Fundamentals 3" exam.
</commit_message>
<xml_diff>
--- a/splunk_certification_path/Splunk Certification Details.xlsx
+++ b/splunk_certification_path/Splunk Certification Details.xlsx
@@ -4,6 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Splunk Fundamentals 1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="Splunk Fundamentals 3" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="149">
   <si>
     <t>Course Name</t>
   </si>
@@ -28,13 +29,26 @@
     <t>Video Link</t>
   </si>
   <si>
+    <t>Splunk Fundamentals 3</t>
+  </si>
+  <si>
     <t>Splunk Fundamentals 1</t>
   </si>
   <si>
+    <t>Splunk Core Certified Consultant</t>
+  </si>
+  <si>
     <t>Splunk Core Certified User</t>
   </si>
   <si>
+    <t>Module 1 – Exploring Statistical Commands</t>
+  </si>
+  <si>
     <t>Module 1 – Introduction</t>
+  </si>
+  <si>
+    <t>Performing statistical analysis with functions 
+of the stat command</t>
   </si>
   <si>
     <t xml:space="preserve">Overview of Buttercup Games Inc.
@@ -48,17 +62,45 @@
 Power User </t>
   </si>
   <si>
+    <t>Using fieldsummary</t>
+  </si>
+  <si>
     <t>Module 2 – What is Splunk?</t>
   </si>
   <si>
     <t>Splunk components</t>
   </si>
   <si>
+    <t>Using appendpipe</t>
+  </si>
+  <si>
+    <t>https://youtu.be/Vjg2UMDuvnA</t>
+  </si>
+  <si>
     <t>https://youtu.be/a-_LHJU07VU</t>
+  </si>
+  <si>
+    <t>Using eventstats</t>
+  </si>
+  <si>
+    <t>https://youtu.be/oD2PIjtLv74
+https://youtu.be/VbdewD-JBr0</t>
   </si>
   <si>
     <t xml:space="preserve">Splunk Enterprise 
 Certified Admin </t>
+  </si>
+  <si>
+    <t>Using streamstats</t>
+  </si>
+  <si>
+    <t>Module 2 – Exploring eval Command Functions</t>
+  </si>
+  <si>
+    <t>Using conversion functions</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ZkMeeFjDiPM</t>
   </si>
   <si>
     <t>Installing Splunk</t>
@@ -95,10 +137,19 @@
 Security Certified Admin</t>
   </si>
   <si>
+    <t>Using data and time functions</t>
+  </si>
+  <si>
     <t>Define Splunk Apps</t>
   </si>
   <si>
+    <t>Using string functions</t>
+  </si>
+  <si>
     <t>https://youtu.be/1lkhVN9DGJU</t>
+  </si>
+  <si>
+    <t>Using comparison and conditional functions</t>
   </si>
   <si>
     <t xml:space="preserve">Splunk IT Service 
@@ -108,13 +159,16 @@
     <t>Customizing your user settings</t>
   </si>
   <si>
-    <t>Splunk Core Certified Consultant</t>
+    <t>Using informational functions</t>
   </si>
   <si>
     <t>Learn basic navigation in Splunk</t>
   </si>
   <si>
     <t>https://youtu.be/Xms0DsuIfq0</t>
+  </si>
+  <si>
+    <t>Using statistical functions</t>
   </si>
   <si>
     <t>Module 4 – Basic Searching</t>
@@ -147,6 +201,9 @@
 </t>
   </si>
   <si>
+    <t>Using mathematical functions</t>
+  </si>
+  <si>
     <t>Save search results</t>
   </si>
   <si>
@@ -168,6 +225,9 @@
   <si>
     <t>Review basic search commands and general search
 practices</t>
+  </si>
+  <si>
+    <t>Using cryptographic functions</t>
   </si>
   <si>
     <t>Examine the search pipeline</t>
@@ -194,10 +254,28 @@
     <t>The top command</t>
   </si>
   <si>
+    <t>Module 3 – Exploring Lookups</t>
+  </si>
+  <si>
+    <t>Including and excluding events based on lookup values</t>
+  </si>
+  <si>
     <t>The rare command</t>
   </si>
   <si>
+    <t>Using KV Store lookups</t>
+  </si>
+  <si>
+    <t>https://youtu.be/1IYezUcNGPY</t>
+  </si>
+  <si>
+    <t>Using external lookups</t>
+  </si>
+  <si>
     <t>The stats command</t>
+  </si>
+  <si>
+    <t>https://youtu.be/DXb5p_EQb_E</t>
   </si>
   <si>
     <t xml:space="preserve">Module 8 – Creating Reports and 
@@ -212,27 +290,125 @@
     <t>https://youtu.be/cdWXKBzPZ78</t>
   </si>
   <si>
+    <t>Using geospatial lookups</t>
+  </si>
+  <si>
+    <t>Using database lookups</t>
+  </si>
+  <si>
+    <t>https://youtu.be/ipi3wJThDic</t>
+  </si>
+  <si>
     <t>Edit reports</t>
+  </si>
+  <si>
+    <t>Understanding best practices for lookups</t>
+  </si>
+  <si>
+    <t>Module 4 – Exploring Alerts</t>
+  </si>
+  <si>
+    <t>Referencing lookups in alerts</t>
+  </si>
+  <si>
+    <t>Outputting alert results to a lookup</t>
+  </si>
+  <si>
+    <t>https://youtu.be/r8g9kRFKvio</t>
   </si>
   <si>
     <t>Create reports that include visualizations such as charts and
 tables</t>
   </si>
   <si>
+    <t>Logging and indexing searchable alert events</t>
+  </si>
+  <si>
+    <t>Using a webhook alert action</t>
+  </si>
+  <si>
+    <t>https://youtu.be/IBgwfJMsXhw</t>
+  </si>
+  <si>
+    <t>Module 5 – Advanced Field Creation and Management</t>
+  </si>
+  <si>
+    <t>Using regex</t>
+  </si>
+  <si>
+    <t>https://youtu.be/LDZ0PKSiuow
+https://youtu.be/ppSxpzK2sj8</t>
+  </si>
+  <si>
+    <t>Using the erex command</t>
+  </si>
+  <si>
     <t xml:space="preserve">Create a dashboard
 </t>
   </si>
   <si>
+    <t>Using the rex command</t>
+  </si>
+  <si>
+    <t>Identifying regex best practices</t>
+  </si>
+  <si>
+    <t>Module 6 – Working with Self-Describing Data and Files</t>
+  </si>
+  <si>
+    <t>Using the spath command</t>
+  </si>
+  <si>
+    <t>https://youtu.be/C3k_v0lzmaM</t>
+  </si>
+  <si>
+    <t>Using the eval command with the spath function</t>
+  </si>
+  <si>
     <t>Add a report to a dashboard</t>
   </si>
   <si>
+    <t>Extracting fields from table-formatted events with multikv</t>
+  </si>
+  <si>
+    <t>https://youtu.be/8kWgDVZZ0GQ</t>
+  </si>
+  <si>
     <t>Edit a dashboard</t>
+  </si>
+  <si>
+    <t>Module 7 – Advanced Search Macros</t>
+  </si>
+  <si>
+    <t>Using nested search macros</t>
+  </si>
+  <si>
+    <t>https://youtu.be/g4v9YZ0sPBE</t>
+  </si>
+  <si>
+    <t>Previewing search macros before executing</t>
+  </si>
+  <si>
+    <t>Using tags and event types in search macros</t>
+  </si>
+  <si>
+    <t>Module 8 – Using Acceleration Options: Reports and 
+Summary Indexing</t>
+  </si>
+  <si>
+    <t>Using report acceleration</t>
+  </si>
+  <si>
+    <t>Using summary indexing</t>
   </si>
   <si>
     <t>Module 9 – Datasets and the 
 Common Information Model</t>
   </si>
   <si>
+    <t>https://youtu.be/joZ3jokt9qs</t>
+  </si>
+  <si>
     <t>Naming conventions</t>
   </si>
   <si>
@@ -249,13 +425,29 @@
     <t xml:space="preserve">Describe lookups </t>
   </si>
   <si>
-    <t>https://youtu.be/1IYezUcNGPY</t>
+    <t>Module 9 – Using Acceleration Options: Data Models 
+and tsidx Files</t>
+  </si>
+  <si>
+    <t>Exploring data models using the datamodel command</t>
+  </si>
+  <si>
+    <t>https://youtu.be/N3FL6rawDLQ</t>
+  </si>
+  <si>
+    <t>Using data model acceleration</t>
   </si>
   <si>
     <t>Create a lookup file and create a lookup definition</t>
   </si>
   <si>
     <t>Configure an automatic lookup</t>
+  </si>
+  <si>
+    <t>Working with tsidx files using the tstats command</t>
+  </si>
+  <si>
+    <t>https://youtu.be/NLPlIiHS1OU</t>
   </si>
   <si>
     <t>Module 11 – Creating Scheduled Reports 
@@ -292,9 +484,6 @@
   </si>
   <si>
     <t>Understand the relationship between data models and pivot</t>
-  </si>
-  <si>
-    <t>https://youtu.be/N3FL6rawDLQ</t>
   </si>
   <si>
     <t>Select a data model object</t>
@@ -322,16 +511,17 @@
     <font>
       <b/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color rgb="FF303030"/>
       <name val="Arial"/>
     </font>
-    <font/>
     <font>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <u/>
       <color rgb="FF0000FF"/>
@@ -385,6 +575,10 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -618,380 +812,380 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
+      <c r="D9" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="C10" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>32</v>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="11">
-      <c r="D11" s="4" t="s">
-        <v>33</v>
+      <c r="D11" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="4" t="s">
-        <v>34</v>
+      <c r="D12" s="3" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="4" t="s">
-        <v>35</v>
+      <c r="D13" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="4" t="s">
-        <v>36</v>
+      <c r="D14" s="3" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15">
-      <c r="D15" s="4" t="s">
-        <v>37</v>
+      <c r="D15" s="3" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="16">
-      <c r="D16" s="4" t="s">
-        <v>38</v>
+      <c r="D16" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17">
-      <c r="D17" s="4" t="s">
-        <v>39</v>
+      <c r="D17" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="18">
-      <c r="D18" s="4" t="s">
-        <v>40</v>
+      <c r="D18" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>42</v>
+      <c r="C19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="20">
-      <c r="D20" s="4" t="s">
-        <v>43</v>
+      <c r="D20" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="21">
-      <c r="D21" s="4" t="s">
-        <v>44</v>
+      <c r="D21" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="22">
       <c r="C22" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>46</v>
+        <v>63</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="23">
-      <c r="D23" s="4" t="s">
-        <v>47</v>
+      <c r="D23" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="24">
-      <c r="D24" s="4" t="s">
-        <v>48</v>
+      <c r="D24" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25">
-      <c r="D25" s="4" t="s">
-        <v>49</v>
+      <c r="D25" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="26">
-      <c r="D26" s="4" t="s">
-        <v>50</v>
+      <c r="D26" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>52</v>
+      <c r="C27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="28">
-      <c r="D28" s="4" t="s">
-        <v>53</v>
+      <c r="D28" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="29">
-      <c r="D29" s="4" t="s">
-        <v>54</v>
+      <c r="D29" s="3" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>56</v>
+      <c r="C30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31">
-      <c r="D31" s="4" t="s">
-        <v>58</v>
+      <c r="D31" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32">
-      <c r="D32" s="4" t="s">
-        <v>59</v>
+      <c r="D32" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33">
-      <c r="D33" s="4" t="s">
-        <v>60</v>
+      <c r="D33" s="3" t="s">
+        <v>100</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34">
-      <c r="D34" s="4" t="s">
-        <v>61</v>
+      <c r="D34" s="3" t="s">
+        <v>107</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35">
-      <c r="D35" s="4" t="s">
-        <v>62</v>
+      <c r="D35" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>57</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36">
-      <c r="C36" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>64</v>
+      <c r="C36" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="37">
-      <c r="D37" s="4" t="s">
-        <v>65</v>
+      <c r="D37" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="38">
       <c r="D38" s="3" t="s">
-        <v>66</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39">
-      <c r="C39" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>68</v>
+      <c r="C39" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40">
-      <c r="D40" s="4" t="s">
-        <v>70</v>
+      <c r="D40" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="41">
-      <c r="D41" s="4" t="s">
-        <v>71</v>
+      <c r="D41" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
     </row>
     <row r="42">
-      <c r="C42" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D42" s="4" t="s">
-        <v>73</v>
+      <c r="C42" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="43">
-      <c r="D43" s="4" t="s">
-        <v>74</v>
+      <c r="D43" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="44">
-      <c r="D44" s="4" t="s">
-        <v>75</v>
+      <c r="D44" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>76</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45">
-      <c r="D45" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>78</v>
+      <c r="D45" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="46">
-      <c r="D46" s="4" t="s">
-        <v>79</v>
+      <c r="D46" s="3" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="47">
-      <c r="C47" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="D47" s="4" t="s">
-        <v>81</v>
+      <c r="C47" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="48">
-      <c r="D48" s="4" t="s">
-        <v>82</v>
+      <c r="D48" s="3" t="s">
+        <v>144</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
     <row r="49">
-      <c r="D49" s="4" t="s">
-        <v>84</v>
+      <c r="D49" s="3" t="s">
+        <v>145</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
     <row r="50">
-      <c r="D50" s="4" t="s">
-        <v>85</v>
+      <c r="D50" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51">
-      <c r="D51" s="4" t="s">
-        <v>86</v>
+      <c r="D51" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="52">
-      <c r="D52" s="4" t="s">
-        <v>87</v>
+      <c r="D52" s="3" t="s">
+        <v>148</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>83</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1015,4 +1209,367 @@
   </hyperlinks>
   <drawing r:id="rId17"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="35.29"/>
+    <col customWidth="1" min="2" max="2" width="44.0"/>
+    <col customWidth="1" min="3" max="3" width="46.14"/>
+    <col customWidth="1" min="4" max="4" width="46.57"/>
+    <col customWidth="1" min="5" max="5" width="36.29"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="D4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="D5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="D8" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="D9" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="D17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="D19" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="D20" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="C21" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="D22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="D23" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="D24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="D26" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="D27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="D28" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="C29" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="D30" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="D31" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="C32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="D33" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="D34" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="C35" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="D36" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="D38" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="D39" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="E4"/>
+    <hyperlink r:id="rId2" ref="E7"/>
+    <hyperlink r:id="rId3" ref="E9"/>
+    <hyperlink r:id="rId4" ref="E10"/>
+    <hyperlink r:id="rId5" ref="E11"/>
+    <hyperlink r:id="rId6" ref="E12"/>
+    <hyperlink r:id="rId7" ref="E13"/>
+    <hyperlink r:id="rId8" ref="E14"/>
+    <hyperlink r:id="rId9" ref="E16"/>
+    <hyperlink r:id="rId10" ref="E17"/>
+    <hyperlink r:id="rId11" ref="E19"/>
+    <hyperlink r:id="rId12" ref="E22"/>
+    <hyperlink r:id="rId13" ref="E24"/>
+    <hyperlink r:id="rId14" ref="E29"/>
+    <hyperlink r:id="rId15" ref="E30"/>
+    <hyperlink r:id="rId16" ref="E31"/>
+    <hyperlink r:id="rId17" ref="E32"/>
+    <hyperlink r:id="rId18" ref="E36"/>
+    <hyperlink r:id="rId19" ref="E37"/>
+    <hyperlink r:id="rId20" ref="E38"/>
+    <hyperlink r:id="rId21" ref="E39"/>
+  </hyperlinks>
+  <drawing r:id="rId22"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
More changes to the certification file
</commit_message>
<xml_diff>
--- a/splunk_certification_path/Splunk Certification Details.xlsx
+++ b/splunk_certification_path/Splunk Certification Details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\YouTube\youtube\splunk_certification_path\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47CB75D4-9A43-4CC4-B6B3-83EC10FCDCC1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA1F626-3743-43BD-8C9D-E379C20E4453}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Splunk Fundamentals 1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Splunk Fundamentals 3" sheetId="3" r:id="rId3"/>
     <sheet name="Advanced Searching &amp; Reporting" sheetId="4" r:id="rId4"/>
     <sheet name="Creating Dashboards with Splunk" sheetId="5" r:id="rId5"/>
+    <sheet name="Building Apps with Splunk" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="326">
   <si>
     <t>Course Name</t>
   </si>
@@ -956,6 +957,99 @@
 https://youtu.be/Z6k4jNUEXO0
 https://youtu.be/hKJdNWtoz_o
 https://youtu.be/O_SogkHGD_U</t>
+  </si>
+  <si>
+    <t>Building Apps with Splunk</t>
+  </si>
+  <si>
+    <t>Module 1 – Planning App Development</t>
+  </si>
+  <si>
+    <t>Create a development environment</t>
+  </si>
+  <si>
+    <t>Improve app performance</t>
+  </si>
+  <si>
+    <t>Identify Splunk log files</t>
+  </si>
+  <si>
+    <t>Use security best practices</t>
+  </si>
+  <si>
+    <t>Create a data generator</t>
+  </si>
+  <si>
+    <t>Module 2 – Creating Apps</t>
+  </si>
+  <si>
+    <t>Define the web framework architecture</t>
+  </si>
+  <si>
+    <t>Identify ways to build Splunk apps</t>
+  </si>
+  <si>
+    <t>Manage apps and add-ons</t>
+  </si>
+  <si>
+    <t>Create an app</t>
+  </si>
+  <si>
+    <t>Configure app properties</t>
+  </si>
+  <si>
+    <t>Create app navigation</t>
+  </si>
+  <si>
+    <t>Module 3 – Adding Data</t>
+  </si>
+  <si>
+    <t>List types of data inputs</t>
+  </si>
+  <si>
+    <t>Identify ways to add data</t>
+  </si>
+  <si>
+    <t>Define when to use a scripted input</t>
+  </si>
+  <si>
+    <t>Create a modular input</t>
+  </si>
+  <si>
+    <t>Module 4 – Using the REST API</t>
+  </si>
+  <si>
+    <t>Explain how the Splunk REST API works</t>
+  </si>
+  <si>
+    <t>Define API endpoints</t>
+  </si>
+  <si>
+    <t>Explain how the KV Store works</t>
+  </si>
+  <si>
+    <t>Create a KV Store</t>
+  </si>
+  <si>
+    <t>Use lookups with a KV Store</t>
+  </si>
+  <si>
+    <t>Module 5 – Packaging Apps</t>
+  </si>
+  <si>
+    <t>Create an app setup screen</t>
+  </si>
+  <si>
+    <t>Define search time precedence</t>
+  </si>
+  <si>
+    <t>Explain local and default differences</t>
+  </si>
+  <si>
+    <t>Package an app</t>
+  </si>
+  <si>
+    <t>https://youtu.be/itBJ47So6tw</t>
   </si>
 </sst>
 </file>
@@ -2866,8 +2960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE5E0D2-D91E-449A-BF17-97A4D52416E7}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="40.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3045,4 +3139,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30698D36-0225-42E0-8290-1D21A27A4DCB}">
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="57" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C2" t="s">
+        <v>296</v>
+      </c>
+      <c r="D2" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D9" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D15" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D16" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>314</v>
+      </c>
+      <c r="D17" t="s">
+        <v>315</v>
+      </c>
+      <c r="E17" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D19" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D20" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D21" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>320</v>
+      </c>
+      <c r="D22" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D23" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="D25" t="s">
+        <v>324</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>